<commit_message>
Changes to grapsh and added text explanations to graphs
</commit_message>
<xml_diff>
--- a/UserCreate.xlsx
+++ b/UserCreate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mado\Documents\C_Desktop\userCharts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D9151B-13FA-4352-8554-23A68247A2DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C78B4D-C384-4F52-AE53-82F80431F5A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CA062317-22C2-486B-A4FE-4A73C795A533}"/>
   </bookViews>
@@ -448,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7B0688-1B2D-4FE5-8F2F-CCF80DE8511D}">
-  <dimension ref="A1:B5391"/>
+  <dimension ref="A1:B5389"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
-      <selection activeCell="B170" sqref="B170"/>
+    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
+      <selection activeCell="E163" sqref="E163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1406,111 +1406,111 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
-        <v>45491</v>
+        <v>45490</v>
       </c>
       <c r="B119" s="4">
-        <v>1553</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
-        <v>45490</v>
+        <v>45489</v>
       </c>
       <c r="B120" s="4">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
-        <v>45489</v>
+        <v>45488</v>
       </c>
       <c r="B121" s="4">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
-        <v>45488</v>
+        <v>45481</v>
       </c>
       <c r="B122" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
-        <v>45481</v>
+        <v>45477</v>
       </c>
       <c r="B123" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
-        <v>45477</v>
+        <v>45474</v>
       </c>
       <c r="B124" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
-        <v>45474</v>
+        <v>45469</v>
       </c>
       <c r="B125" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
-        <v>45469</v>
+        <v>45468</v>
       </c>
       <c r="B126" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
-        <v>45468</v>
+        <v>45467</v>
       </c>
       <c r="B127" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
-        <v>45467</v>
+        <v>45462</v>
       </c>
       <c r="B128" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
-        <v>45462</v>
+        <v>45460</v>
       </c>
       <c r="B129" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
-        <v>45460</v>
+        <v>45455</v>
       </c>
       <c r="B130" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
-        <v>45455</v>
+        <v>45453</v>
       </c>
       <c r="B131" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
-        <v>45453</v>
+        <v>45449</v>
       </c>
       <c r="B132" s="4">
         <v>1</v>
@@ -1518,7 +1518,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
-        <v>45449</v>
+        <v>45439</v>
       </c>
       <c r="B133" s="4">
         <v>1</v>
@@ -1526,23 +1526,23 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
-        <v>45439</v>
+        <v>45435</v>
       </c>
       <c r="B134" s="4">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
-        <v>45435</v>
+        <v>45433</v>
       </c>
       <c r="B135" s="4">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
-        <v>45433</v>
+        <v>45429</v>
       </c>
       <c r="B136" s="4">
         <v>1</v>
@@ -1550,47 +1550,47 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
-        <v>45429</v>
+        <v>45428</v>
       </c>
       <c r="B137" s="4">
-        <v>1</v>
+        <v>32</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
-        <v>45428</v>
+        <v>45427</v>
       </c>
       <c r="B138" s="4">
-        <v>32</v>
+        <v>2</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
-        <v>45427</v>
+        <v>45425</v>
       </c>
       <c r="B139" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
-        <v>45425</v>
+        <v>45422</v>
       </c>
       <c r="B140" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
-        <v>45422</v>
+        <v>45413</v>
       </c>
       <c r="B141" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
-        <v>45413</v>
+        <v>45412</v>
       </c>
       <c r="B142" s="4">
         <v>1</v>
@@ -1598,47 +1598,47 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
-        <v>45412</v>
+        <v>45411</v>
       </c>
       <c r="B143" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
-        <v>45411</v>
+        <v>45408</v>
       </c>
       <c r="B144" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
-        <v>45408</v>
+        <v>45407</v>
       </c>
       <c r="B145" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
-        <v>45407</v>
+        <v>45406</v>
       </c>
       <c r="B146" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
-        <v>45406</v>
+        <v>45404</v>
       </c>
       <c r="B147" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
-        <v>45404</v>
+        <v>45401</v>
       </c>
       <c r="B148" s="4">
         <v>2</v>
@@ -1646,39 +1646,39 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
-        <v>45401</v>
+        <v>45400</v>
       </c>
       <c r="B149" s="4">
-        <v>2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
-        <v>45400</v>
+        <v>45397</v>
       </c>
       <c r="B150" s="4">
-        <v>16</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
-        <v>45397</v>
+        <v>45391</v>
       </c>
       <c r="B151" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
-        <v>45391</v>
+        <v>45386</v>
       </c>
       <c r="B152" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
-        <v>45386</v>
+        <v>45384</v>
       </c>
       <c r="B153" s="4">
         <v>1</v>
@@ -1686,63 +1686,63 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
-        <v>45384</v>
+        <v>45379</v>
       </c>
       <c r="B154" s="4">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
-        <v>45379</v>
+        <v>45378</v>
       </c>
       <c r="B155" s="4">
-        <v>24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
-        <v>45378</v>
+        <v>45377</v>
       </c>
       <c r="B156" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
-        <v>45377</v>
+        <v>45376</v>
       </c>
       <c r="B157" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
-        <v>45376</v>
+        <v>45373</v>
       </c>
       <c r="B158" s="4">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
-        <v>45373</v>
+        <v>45369</v>
       </c>
       <c r="B159" s="4">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
-        <v>45372</v>
+        <v>45356</v>
       </c>
       <c r="B160" s="4">
-        <v>2520</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
-        <v>45369</v>
+        <v>45313</v>
       </c>
       <c r="B161" s="4">
         <v>1</v>
@@ -1750,29 +1750,19 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
-        <v>45356</v>
+        <v>45301</v>
       </c>
       <c r="B162" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="3">
-        <v>45313</v>
-      </c>
-      <c r="B163" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="3">
-        <v>45301</v>
-      </c>
-      <c r="B164" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="167" spans="1:2" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A169" s="5"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A170" s="5"/>
+    </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="5"/>
     </row>
@@ -17430,13 +17420,8 @@
     <row r="5389" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5389" s="5"/>
     </row>
-    <row r="5390" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5390" s="5"/>
-    </row>
-    <row r="5391" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5391" s="5"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>